<commit_message>
update porous flow file
</commit_message>
<xml_diff>
--- a/SUBSLIDE/MPMICE2/porousFlow/PorousFlow.xlsx
+++ b/SUBSLIDE/MPMICE2/porousFlow/PorousFlow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uintah\Uintah_NTNU\SUBSLIDE\MPMICE2\porousFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B601F135-182A-40AF-B31E-5B55733ABC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E96643-A082-40DA-9843-36ED27FBC34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Analytical solution</t>
   </si>
@@ -79,13 +79,16 @@
     <t>Analytical solution vs numerical solution</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>m/s</t>
   </si>
   <si>
     <t>cm/s</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>Permeability</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,6 +171,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1939,9 +1960,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P11"/>
+  <dimension ref="B2:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1967,24 +1988,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="J2" s="7" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="J2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -1999,32 +2020,32 @@
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5" t="s">
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="9"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
-        <v>1.0000000000000001E-5</v>
+        <v>1.83E-2</v>
       </c>
       <c r="C5" s="3">
         <v>0.44</v>
@@ -2035,15 +2056,15 @@
       <c r="E5" s="3">
         <v>1E-3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="7">
         <v>101325</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="7">
         <v>1</v>
       </c>
       <c r="H5" s="2">
         <f>1/C5*B5*B5/180/E5*(1-D5)^3/D5/D5*F5/G5</f>
-        <v>3.4751488095238082E-5</v>
+        <v>116.3792584821428</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>3</v>
@@ -2114,9 +2135,10 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="8"/>
       <c r="J8" s="2">
         <v>0.66</v>
       </c>
@@ -2140,12 +2162,12 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+      <c r="B9" s="8">
         <f>B5*B5/180/E5*(1-D5)^3/D5/D5</f>
-        <v>1.50907029478458E-10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>5.0537255102040782E-4</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="J9" s="2">
         <v>0.64</v>
@@ -2172,10 +2194,10 @@
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <f>B9*100</f>
-        <v>1.50907029478458E-8</v>
+        <v>5.0537255102040782E-2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="2">
         <v>0.62</v>
@@ -2223,6 +2245,57 @@
       </c>
       <c r="P11" s="2">
         <v>6.4199999999999993E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="C20" s="6">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>8.5000000000000006E-5</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1E-8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1.5090702947845799E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>1.83E-3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5.0537255102040782E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5.0765124716553246E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>